<commit_message>
modify flute base and piccolo mapping
</commit_message>
<xml_diff>
--- a/Fingering.xlsx
+++ b/Fingering.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eduardo/projects/personal/fingering-diagram/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D0D95AD-9D93-3049-B1A8-B3269D499D25}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{640FF0CD-9ECC-FD4A-B9F7-2DA860C560D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34460" yWindow="1980" windowWidth="33600" windowHeight="18880" activeTab="3" xr2:uid="{851DC363-32CE-4241-A25E-21E01B6D35D5}"/>
+    <workbookView xWindow="34460" yWindow="1980" windowWidth="33600" windowHeight="18880" activeTab="1" xr2:uid="{851DC363-32CE-4241-A25E-21E01B6D35D5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sections" sheetId="6" r:id="rId1"/>
@@ -226,10 +226,9 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
-          <t>https://www.dolmetsch.com/textfingeringchart.htm
-http://www.recorder-fingerings.com/en/F.php?t=aBar.1S.3a</t>
+          <t xml:space="preserve">https://www.dolmetsch.com/textfingeringchart.htm
+</t>
         </r>
         <r>
           <rPr>
@@ -238,7 +237,7 @@
             <rFont val="Calibri"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">
+          <t xml:space="preserve">http://www.recorder-fingerings.com/en/F.php?t=aBar.1S.3a
 </t>
         </r>
         <r>
@@ -257,18 +256,8 @@
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
             <family val="2"/>
-            <scheme val="minor"/>
           </rPr>
-          <t>http://www.flute-a-bec.com/tablaturgb.html</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
+          <t xml:space="preserve">http://www.flute-a-bec.com/tablaturgb.html
 </t>
         </r>
         <r>
@@ -297,7 +286,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="785" uniqueCount="201">
   <si>
     <t>B3</t>
   </si>
@@ -899,10 +888,7 @@
     <t>\uEF9D</t>
   </si>
   <si>
-    <t>Fingering</t>
-  </si>
-  <si>
-    <t>=</t>
+    <t>\uEF60</t>
   </si>
 </sst>
 </file>
@@ -913,7 +899,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -974,13 +960,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="12"/>
       <name val="Calibri"/>
@@ -1024,7 +1003,7 @@
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1404,7 +1383,7 @@
         <v>181</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:C7" si="1">C3+160</f>
+        <f t="shared" ref="C4:C6" si="1">C3+160</f>
         <v>60800</v>
       </c>
       <c r="D4" t="str">
@@ -1495,11 +1474,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD8F6977-9827-D446-AF50-2B67C7CC719C}">
   <dimension ref="A1:Z54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C19" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1593,7 +1572,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B2" s="4"/>
       <c r="C2" s="4" t="s">
         <v>153</v>
@@ -1654,12 +1633,12 @@
       <c r="X2" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="Y2" s="8" t="str">
+      <c r="Y2" s="3" t="str">
         <f>"\uEC40\uEC41\uEC42"</f>
         <v>\uEC40\uEC41\uEC42</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1703,7 +1682,7 @@
       <c r="X3" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="Y3" s="8" t="str">
+      <c r="Y3" s="3" t="str">
         <f>_xlfn.CONCAT(C3:U3)</f>
         <v>\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC4F\uEC51\uEC54\uEC55\uEC53</v>
       </c>
@@ -1712,7 +1691,7 @@
         <v>'\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC4F\uEC51\uEC54\uEC55\uEC53',</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1752,7 +1731,7 @@
       <c r="X4" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="Y4" s="8" t="str">
+      <c r="Y4" s="3" t="str">
         <f t="shared" ref="Y4:Y40" si="0">_xlfn.CONCAT(C4:U4)</f>
         <v>\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC4F\uEC51\uEC55\uEC53</v>
       </c>
@@ -1761,7 +1740,7 @@
         <v>'\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC4F\uEC51\uEC54\uEC55\uEC53','\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC4F\uEC51\uEC55\uEC53',</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>38</v>
       </c>
@@ -1798,7 +1777,7 @@
       <c r="X5" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="Y5" s="8" t="str">
+      <c r="Y5" s="3" t="str">
         <f t="shared" si="0"/>
         <v>\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC4F\uEC51\uEC53</v>
       </c>
@@ -1807,7 +1786,7 @@
         <v>'\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC4F\uEC51\uEC54\uEC55\uEC53','\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC4F\uEC51\uEC55\uEC53','\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC4F\uEC51\uEC53',</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -1846,7 +1825,7 @@
       <c r="X6" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="Y6" s="8" t="str">
+      <c r="Y6" s="3" t="str">
         <f t="shared" si="0"/>
         <v>\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC4F\uEC51</v>
       </c>
@@ -1855,7 +1834,7 @@
         <v>'\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC4F\uEC51\uEC54\uEC55\uEC53','\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC4F\uEC51\uEC55\uEC53','\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC4F\uEC51\uEC53','\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC4F\uEC51',</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>39</v>
       </c>
@@ -1896,7 +1875,7 @@
       <c r="X7" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="Y7" s="8" t="str">
+      <c r="Y7" s="3" t="str">
         <f t="shared" si="0"/>
         <v>\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC4F\uEC51\uEC52</v>
       </c>
@@ -1905,7 +1884,7 @@
         <v>'\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC4F\uEC51\uEC54\uEC55\uEC53','\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC4F\uEC51\uEC55\uEC53','\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC4F\uEC51\uEC53','\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC4F\uEC51','\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC4F\uEC51\uEC52',</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -1944,7 +1923,7 @@
       <c r="X8" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="Y8" s="8" t="str">
+      <c r="Y8" s="3" t="str">
         <f t="shared" si="0"/>
         <v>\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC4F\uEC52</v>
       </c>
@@ -1953,7 +1932,7 @@
         <v>'\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC4F\uEC51\uEC54\uEC55\uEC53','\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC4F\uEC51\uEC55\uEC53','\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC4F\uEC51\uEC53','\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC4F\uEC51','\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC4F\uEC51\uEC52','\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC4F\uEC52',</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -1990,7 +1969,7 @@
       <c r="X9" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="Y9" s="8" t="str">
+      <c r="Y9" s="3" t="str">
         <f t="shared" si="0"/>
         <v>\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC52</v>
       </c>
@@ -1999,7 +1978,7 @@
         <v>'\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC4F\uEC51\uEC54\uEC55\uEC53','\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC4F\uEC51\uEC55\uEC53','\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC4F\uEC51\uEC53','\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC4F\uEC51','\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC4F\uEC51\uEC52','\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC4F\uEC52','\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC52',</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>40</v>
       </c>
@@ -2035,7 +2014,7 @@
       <c r="X10" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="Y10" s="8" t="str">
+      <c r="Y10" s="3" t="str">
         <f t="shared" si="0"/>
         <v>\uEC46\uEC47\uEC48\uEC49\uEC51\uEC52</v>
       </c>
@@ -2044,7 +2023,7 @@
         <v>'\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC4F\uEC51\uEC54\uEC55\uEC53','\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC4F\uEC51\uEC55\uEC53','\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC4F\uEC51\uEC53','\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC4F\uEC51','\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC4F\uEC51\uEC52','\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC4F\uEC52','\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC52','\uEC46\uEC47\uEC48\uEC49\uEC51\uEC52',</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -2078,7 +2057,7 @@
       <c r="X11" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="Y11" s="8" t="str">
+      <c r="Y11" s="3" t="str">
         <f t="shared" si="0"/>
         <v>\uEC46\uEC47\uEC48\uEC49\uEC52</v>
       </c>
@@ -2087,7 +2066,7 @@
         <v>'\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC4F\uEC51\uEC54\uEC55\uEC53','\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC4F\uEC51\uEC55\uEC53','\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC4F\uEC51\uEC53','\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC4F\uEC51','\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC4F\uEC51\uEC52','\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC4F\uEC52','\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC52','\uEC46\uEC47\uEC48\uEC49\uEC51\uEC52','\uEC46\uEC47\uEC48\uEC49\uEC52',</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>41</v>
       </c>
@@ -2123,7 +2102,7 @@
       <c r="X12" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="Y12" s="8" t="str">
+      <c r="Y12" s="3" t="str">
         <f t="shared" si="0"/>
         <v>\uEC46\uEC47\uEC48\uEC49\uEC4A\uEC52</v>
       </c>
@@ -2132,7 +2111,7 @@
         <v>'\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC4F\uEC51\uEC54\uEC55\uEC53','\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC4F\uEC51\uEC55\uEC53','\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC4F\uEC51\uEC53','\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC4F\uEC51','\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC4F\uEC51\uEC52','\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC4F\uEC52','\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC52','\uEC46\uEC47\uEC48\uEC49\uEC51\uEC52','\uEC46\uEC47\uEC48\uEC49\uEC52','\uEC46\uEC47\uEC48\uEC49\uEC4A\uEC52',</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -2164,7 +2143,7 @@
       <c r="X13" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="Y13" s="8" t="str">
+      <c r="Y13" s="3" t="str">
         <f t="shared" si="0"/>
         <v>\uEC46\uEC47\uEC48\uEC52</v>
       </c>
@@ -2173,7 +2152,7 @@
         <v>'\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC4F\uEC51\uEC54\uEC55\uEC53','\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC4F\uEC51\uEC55\uEC53','\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC4F\uEC51\uEC53','\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC4F\uEC51','\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC4F\uEC51\uEC52','\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC4F\uEC52','\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC52','\uEC46\uEC47\uEC48\uEC49\uEC51\uEC52','\uEC46\uEC47\uEC48\uEC49\uEC52','\uEC46\uEC47\uEC48\uEC49\uEC4A\uEC52','\uEC46\uEC47\uEC48\uEC52',</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>42</v>
       </c>
@@ -2205,7 +2184,7 @@
       <c r="X14" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="Y14" s="8" t="str">
+      <c r="Y14" s="3" t="str">
         <f t="shared" si="0"/>
         <v>\uEC46\uEC47\uEC4D\uEC52</v>
       </c>
@@ -2214,7 +2193,7 @@
         <v>'\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC4F\uEC51\uEC54\uEC55\uEC53','\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC4F\uEC51\uEC55\uEC53','\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC4F\uEC51\uEC53','\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC4F\uEC51','\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC4F\uEC51\uEC52','\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC4F\uEC52','\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC52','\uEC46\uEC47\uEC48\uEC49\uEC51\uEC52','\uEC46\uEC47\uEC48\uEC49\uEC52','\uEC46\uEC47\uEC48\uEC49\uEC4A\uEC52','\uEC46\uEC47\uEC48\uEC52','\uEC46\uEC47\uEC4D\uEC52',</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -2244,7 +2223,7 @@
       <c r="X15" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="Y15" s="8" t="str">
+      <c r="Y15" s="3" t="str">
         <f t="shared" si="0"/>
         <v>\uEC46\uEC47\uEC52</v>
       </c>
@@ -2253,7 +2232,7 @@
         <v>'\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC4F\uEC51\uEC54\uEC55\uEC53','\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC4F\uEC51\uEC55\uEC53','\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC4F\uEC51\uEC53','\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC4F\uEC51','\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC4F\uEC51\uEC52','\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC4F\uEC52','\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC52','\uEC46\uEC47\uEC48\uEC49\uEC51\uEC52','\uEC46\uEC47\uEC48\uEC49\uEC52','\uEC46\uEC47\uEC48\uEC49\uEC4A\uEC52','\uEC46\uEC47\uEC48\uEC52','\uEC46\uEC47\uEC4D\uEC52','\uEC46\uEC47\uEC52',</v>
       </c>
     </row>
-    <row r="16" spans="1:26" ht="18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>27</v>
       </c>
@@ -2281,7 +2260,7 @@
       <c r="X16" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="Y16" s="8" t="str">
+      <c r="Y16" s="3" t="str">
         <f t="shared" si="0"/>
         <v>\uEC47\uEC52</v>
       </c>
@@ -2290,7 +2269,7 @@
         <v>'\uEC47\uEC52',</v>
       </c>
     </row>
-    <row r="17" spans="1:26" ht="18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>43</v>
       </c>
@@ -2316,7 +2295,7 @@
       <c r="X17" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="Y17" s="8" t="str">
+      <c r="Y17" s="3" t="str">
         <f t="shared" si="0"/>
         <v>\uEC52</v>
       </c>
@@ -2325,7 +2304,7 @@
         <v>'\uEC47\uEC52','\uEC52',</v>
       </c>
     </row>
-    <row r="18" spans="1:26" ht="18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -2361,7 +2340,7 @@
       <c r="X18" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="Y18" s="8" t="str">
+      <c r="Y18" s="3" t="str">
         <f t="shared" si="0"/>
         <v>\uEC46\uEC48\uEC49\uEC4D\uEC4F\uEC51</v>
       </c>
@@ -2370,7 +2349,7 @@
         <v>'\uEC47\uEC52','\uEC52','\uEC46\uEC48\uEC49\uEC4D\uEC4F\uEC51',</v>
       </c>
     </row>
-    <row r="19" spans="1:26" ht="18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>44</v>
       </c>
@@ -2408,7 +2387,7 @@
       <c r="X19" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="Y19" s="8" t="str">
+      <c r="Y19" s="3" t="str">
         <f t="shared" si="0"/>
         <v>\uEC46\uEC48\uEC49\uEC4D\uEC4F\uEC51\uEC52</v>
       </c>
@@ -2417,7 +2396,7 @@
         <v>'\uEC47\uEC52','\uEC52','\uEC46\uEC48\uEC49\uEC4D\uEC4F\uEC51','\uEC46\uEC48\uEC49\uEC4D\uEC4F\uEC51\uEC52',</v>
       </c>
     </row>
-    <row r="20" spans="1:26" ht="18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -2455,7 +2434,7 @@
       <c r="X20" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="Y20" s="8" t="str">
+      <c r="Y20" s="3" t="str">
         <f t="shared" si="0"/>
         <v>\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC4F\uEC52</v>
       </c>
@@ -2464,7 +2443,7 @@
         <v>'\uEC47\uEC52','\uEC52','\uEC46\uEC48\uEC49\uEC4D\uEC4F\uEC51','\uEC46\uEC48\uEC49\uEC4D\uEC4F\uEC51\uEC52','\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC4F\uEC52',</v>
       </c>
     </row>
-    <row r="21" spans="1:26" ht="18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -2500,7 +2479,7 @@
       <c r="X21" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="Y21" s="8" t="str">
+      <c r="Y21" s="3" t="str">
         <f t="shared" si="0"/>
         <v>\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC52</v>
       </c>
@@ -2509,7 +2488,7 @@
         <v>'\uEC47\uEC52','\uEC52','\uEC46\uEC48\uEC49\uEC4D\uEC4F\uEC51','\uEC46\uEC48\uEC49\uEC4D\uEC4F\uEC51\uEC52','\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC4F\uEC52','\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC52',</v>
       </c>
     </row>
-    <row r="22" spans="1:26" ht="18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>45</v>
       </c>
@@ -2545,7 +2524,7 @@
       <c r="X22" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="Y22" s="8" t="str">
+      <c r="Y22" s="3" t="str">
         <f t="shared" si="0"/>
         <v>\uEC46\uEC47\uEC48\uEC49\uEC51\uEC52</v>
       </c>
@@ -2554,7 +2533,7 @@
         <v>'\uEC47\uEC52','\uEC52','\uEC46\uEC48\uEC49\uEC4D\uEC4F\uEC51','\uEC46\uEC48\uEC49\uEC4D\uEC4F\uEC51\uEC52','\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC4F\uEC52','\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC52','\uEC46\uEC47\uEC48\uEC49\uEC51\uEC52',</v>
       </c>
     </row>
-    <row r="23" spans="1:26" ht="18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>17</v>
       </c>
@@ -2588,7 +2567,7 @@
       <c r="X23" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="Y23" s="8" t="str">
+      <c r="Y23" s="3" t="str">
         <f t="shared" si="0"/>
         <v>\uEC46\uEC47\uEC48\uEC49\uEC52</v>
       </c>
@@ -2597,7 +2576,7 @@
         <v>'\uEC47\uEC52','\uEC52','\uEC46\uEC48\uEC49\uEC4D\uEC4F\uEC51','\uEC46\uEC48\uEC49\uEC4D\uEC4F\uEC51\uEC52','\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC4F\uEC52','\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC52','\uEC46\uEC47\uEC48\uEC49\uEC51\uEC52','\uEC46\uEC47\uEC48\uEC49\uEC52',</v>
       </c>
     </row>
-    <row r="24" spans="1:26" ht="18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>46</v>
       </c>
@@ -2633,7 +2612,7 @@
       <c r="X24" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="Y24" s="8" t="str">
+      <c r="Y24" s="3" t="str">
         <f t="shared" si="0"/>
         <v>\uEC46\uEC47\uEC48\uEC49\uEC4A\uEC52</v>
       </c>
@@ -2642,7 +2621,7 @@
         <v>'\uEC47\uEC52','\uEC52','\uEC46\uEC48\uEC49\uEC4D\uEC4F\uEC51','\uEC46\uEC48\uEC49\uEC4D\uEC4F\uEC51\uEC52','\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC4F\uEC52','\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC52','\uEC46\uEC47\uEC48\uEC49\uEC51\uEC52','\uEC46\uEC47\uEC48\uEC49\uEC52','\uEC46\uEC47\uEC48\uEC49\uEC4A\uEC52',</v>
       </c>
     </row>
-    <row r="25" spans="1:26" ht="18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>16</v>
       </c>
@@ -2674,7 +2653,7 @@
       <c r="X25" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="Y25" s="8" t="str">
+      <c r="Y25" s="3" t="str">
         <f t="shared" si="0"/>
         <v>\uEC46\uEC47\uEC48\uEC52</v>
       </c>
@@ -2683,7 +2662,7 @@
         <v>'\uEC47\uEC52','\uEC52','\uEC46\uEC48\uEC49\uEC4D\uEC4F\uEC51','\uEC46\uEC48\uEC49\uEC4D\uEC4F\uEC51\uEC52','\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC4F\uEC52','\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC52','\uEC46\uEC47\uEC48\uEC49\uEC51\uEC52','\uEC46\uEC47\uEC48\uEC49\uEC52','\uEC46\uEC47\uEC48\uEC49\uEC4A\uEC52','\uEC46\uEC47\uEC48\uEC52',</v>
       </c>
     </row>
-    <row r="26" spans="1:26" ht="18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>47</v>
       </c>
@@ -2715,7 +2694,7 @@
       <c r="X26" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="Y26" s="8" t="str">
+      <c r="Y26" s="3" t="str">
         <f t="shared" si="0"/>
         <v>\uEC46\uEC47\uEC4D\uEC52</v>
       </c>
@@ -2724,7 +2703,7 @@
         <v>'\uEC47\uEC52','\uEC52','\uEC46\uEC48\uEC49\uEC4D\uEC4F\uEC51','\uEC46\uEC48\uEC49\uEC4D\uEC4F\uEC51\uEC52','\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC4F\uEC52','\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC52','\uEC46\uEC47\uEC48\uEC49\uEC51\uEC52','\uEC46\uEC47\uEC48\uEC49\uEC52','\uEC46\uEC47\uEC48\uEC49\uEC4A\uEC52','\uEC46\uEC47\uEC48\uEC52','\uEC46\uEC47\uEC4D\uEC52',</v>
       </c>
     </row>
-    <row r="27" spans="1:26" ht="18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>15</v>
       </c>
@@ -2754,7 +2733,7 @@
       <c r="X27" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="Y27" s="8" t="str">
+      <c r="Y27" s="3" t="str">
         <f t="shared" si="0"/>
         <v>\uEC46\uEC47\uEC52</v>
       </c>
@@ -2763,7 +2742,7 @@
         <v>'\uEC47\uEC52','\uEC52','\uEC46\uEC48\uEC49\uEC4D\uEC4F\uEC51','\uEC46\uEC48\uEC49\uEC4D\uEC4F\uEC51\uEC52','\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC4F\uEC52','\uEC46\uEC47\uEC48\uEC49\uEC4D\uEC52','\uEC46\uEC47\uEC48\uEC49\uEC51\uEC52','\uEC46\uEC47\uEC48\uEC49\uEC52','\uEC46\uEC47\uEC48\uEC49\uEC4A\uEC52','\uEC46\uEC47\uEC48\uEC52','\uEC46\uEC47\uEC4D\uEC52','\uEC46\uEC47\uEC52',</v>
       </c>
     </row>
-    <row r="28" spans="1:26" ht="18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -2791,7 +2770,7 @@
       <c r="X28" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="Y28" s="8" t="str">
+      <c r="Y28" s="3" t="str">
         <f t="shared" si="0"/>
         <v>\uEC47\uEC52</v>
       </c>
@@ -2800,7 +2779,7 @@
         <v>'\uEC47\uEC52',</v>
       </c>
     </row>
-    <row r="29" spans="1:26" ht="18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>48</v>
       </c>
@@ -2826,7 +2805,7 @@
       <c r="X29" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="Y29" s="8" t="str">
+      <c r="Y29" s="3" t="str">
         <f t="shared" si="0"/>
         <v>\uEC52</v>
       </c>
@@ -2835,7 +2814,7 @@
         <v>'\uEC47\uEC52','\uEC52',</v>
       </c>
     </row>
-    <row r="30" spans="1:26" ht="18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>14</v>
       </c>
@@ -2867,7 +2846,7 @@
       <c r="X30" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="Y30" s="8" t="str">
+      <c r="Y30" s="3" t="str">
         <f t="shared" si="0"/>
         <v>\uEC46\uEC48\uEC49\uEC52</v>
       </c>
@@ -2876,7 +2855,7 @@
         <v>'\uEC47\uEC52','\uEC52','\uEC46\uEC48\uEC49\uEC52',</v>
       </c>
     </row>
-    <row r="31" spans="1:26" ht="18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>49</v>
       </c>
@@ -2918,7 +2897,7 @@
       <c r="X31" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="Y31" s="8" t="str">
+      <c r="Y31" s="3" t="str">
         <f t="shared" si="0"/>
         <v>\uEC46\uEC47\uEC48\uEC49\uEC4A\uEC4D\uEC4F\uEC51\uEC52</v>
       </c>
@@ -2927,7 +2906,7 @@
         <v>'\uEC47\uEC52','\uEC52','\uEC46\uEC48\uEC49\uEC52','\uEC46\uEC47\uEC48\uEC49\uEC4A\uEC4D\uEC4F\uEC51\uEC52',</v>
       </c>
     </row>
-    <row r="32" spans="1:26" ht="18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>13</v>
       </c>
@@ -2963,7 +2942,7 @@
       <c r="X32" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="Y32" s="8" t="str">
+      <c r="Y32" s="3" t="str">
         <f t="shared" si="0"/>
         <v>\uEC46\uEC47\uEC48\uEC4D\uEC4F\uEC52</v>
       </c>
@@ -2972,7 +2951,7 @@
         <v>'\uEC47\uEC52','\uEC52','\uEC46\uEC48\uEC49\uEC52','\uEC46\uEC47\uEC48\uEC49\uEC4A\uEC4D\uEC4F\uEC51\uEC52','\uEC46\uEC47\uEC48\uEC4D\uEC4F\uEC52',</v>
       </c>
     </row>
-    <row r="33" spans="1:26" ht="18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>12</v>
       </c>
@@ -3006,7 +2985,7 @@
       <c r="X33" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="Y33" s="8" t="str">
+      <c r="Y33" s="3" t="str">
         <f t="shared" si="0"/>
         <v>\uEC46\uEC47\uEC49\uEC4D\uEC52</v>
       </c>
@@ -3015,7 +2994,7 @@
         <v>'\uEC47\uEC52','\uEC52','\uEC46\uEC48\uEC49\uEC52','\uEC46\uEC47\uEC48\uEC49\uEC4A\uEC4D\uEC4F\uEC51\uEC52','\uEC46\uEC47\uEC48\uEC4D\uEC4F\uEC52','\uEC46\uEC47\uEC49\uEC4D\uEC52',</v>
       </c>
     </row>
-    <row r="34" spans="1:26" ht="18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>50</v>
       </c>
@@ -3049,7 +3028,7 @@
       <c r="X34" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="Y34" s="8" t="str">
+      <c r="Y34" s="3" t="str">
         <f t="shared" si="0"/>
         <v>\uEC46\uEC47\uEC49\uEC51\uEC52</v>
       </c>
@@ -3058,7 +3037,7 @@
         <v>'\uEC47\uEC52','\uEC52','\uEC46\uEC48\uEC49\uEC52','\uEC46\uEC47\uEC48\uEC49\uEC4A\uEC4D\uEC4F\uEC51\uEC52','\uEC46\uEC47\uEC48\uEC4D\uEC4F\uEC52','\uEC46\uEC47\uEC49\uEC4D\uEC52','\uEC46\uEC47\uEC49\uEC51\uEC52',</v>
       </c>
     </row>
-    <row r="35" spans="1:26" ht="18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>11</v>
       </c>
@@ -3090,7 +3069,7 @@
       <c r="X35" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="Y35" s="8" t="str">
+      <c r="Y35" s="3" t="str">
         <f t="shared" si="0"/>
         <v>\uEC47\uEC48\uEC49\uEC52</v>
       </c>
@@ -3099,7 +3078,7 @@
         <v>'\uEC47\uEC52','\uEC52','\uEC46\uEC48\uEC49\uEC52','\uEC46\uEC47\uEC48\uEC49\uEC4A\uEC4D\uEC4F\uEC51\uEC52','\uEC46\uEC47\uEC48\uEC4D\uEC4F\uEC52','\uEC46\uEC47\uEC49\uEC4D\uEC52','\uEC46\uEC47\uEC49\uEC51\uEC52','\uEC47\uEC48\uEC49\uEC52',</v>
       </c>
     </row>
-    <row r="36" spans="1:26" ht="18" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>51</v>
       </c>
@@ -3131,7 +3110,7 @@
       <c r="X36" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="Y36" s="8" t="str">
+      <c r="Y36" s="3" t="str">
         <f t="shared" si="0"/>
         <v>\uEC48\uEC49\uEC4A\uEC52</v>
       </c>
@@ -3140,7 +3119,7 @@
         <v>'\uEC47\uEC52','\uEC52','\uEC46\uEC48\uEC49\uEC52','\uEC46\uEC47\uEC48\uEC49\uEC4A\uEC4D\uEC4F\uEC51\uEC52','\uEC46\uEC47\uEC48\uEC4D\uEC4F\uEC52','\uEC46\uEC47\uEC49\uEC4D\uEC52','\uEC46\uEC47\uEC49\uEC51\uEC52','\uEC47\uEC48\uEC49\uEC52','\uEC48\uEC49\uEC4A\uEC52',</v>
       </c>
     </row>
-    <row r="37" spans="1:26" ht="18" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>10</v>
       </c>
@@ -3172,7 +3151,7 @@
       <c r="X37" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="Y37" s="8" t="str">
+      <c r="Y37" s="3" t="str">
         <f t="shared" si="0"/>
         <v>\uEC46\uEC48\uEC4D\uEC52</v>
       </c>
@@ -3181,7 +3160,7 @@
         <v>'\uEC47\uEC52','\uEC52','\uEC46\uEC48\uEC49\uEC52','\uEC46\uEC47\uEC48\uEC49\uEC4A\uEC4D\uEC4F\uEC51\uEC52','\uEC46\uEC47\uEC48\uEC4D\uEC4F\uEC52','\uEC46\uEC47\uEC49\uEC4D\uEC52','\uEC46\uEC47\uEC49\uEC51\uEC52','\uEC47\uEC48\uEC49\uEC52','\uEC48\uEC49\uEC4A\uEC52','\uEC46\uEC48\uEC4D\uEC52',</v>
       </c>
     </row>
-    <row r="38" spans="1:26" ht="18" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>52</v>
       </c>
@@ -3211,7 +3190,7 @@
       <c r="X38" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="Y38" s="8" t="str">
+      <c r="Y38" s="3" t="str">
         <f t="shared" si="0"/>
         <v>\uEC46\uEC4E\uEC4D</v>
       </c>
@@ -3220,7 +3199,7 @@
         <v>'\uEC47\uEC52','\uEC52','\uEC46\uEC48\uEC49\uEC52','\uEC46\uEC47\uEC48\uEC49\uEC4A\uEC4D\uEC4F\uEC51\uEC52','\uEC46\uEC47\uEC48\uEC4D\uEC4F\uEC52','\uEC46\uEC47\uEC49\uEC4D\uEC52','\uEC46\uEC47\uEC49\uEC51\uEC52','\uEC47\uEC48\uEC49\uEC52','\uEC48\uEC49\uEC4A\uEC52','\uEC46\uEC48\uEC4D\uEC52','\uEC46\uEC4E\uEC4D',</v>
       </c>
     </row>
-    <row r="39" spans="1:26" ht="18" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>9</v>
       </c>
@@ -3251,7 +3230,7 @@
       <c r="X39" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="Y39" s="8" t="str">
+      <c r="Y39" s="3" t="str">
         <f t="shared" si="0"/>
         <v>\uEC46\uEC47\uEC49\uEC50</v>
       </c>
@@ -3260,7 +3239,7 @@
         <v>'\uEC47\uEC52','\uEC52','\uEC46\uEC48\uEC49\uEC52','\uEC46\uEC47\uEC48\uEC49\uEC4A\uEC4D\uEC4F\uEC51\uEC52','\uEC46\uEC47\uEC48\uEC4D\uEC4F\uEC52','\uEC46\uEC47\uEC49\uEC4D\uEC52','\uEC46\uEC47\uEC49\uEC51\uEC52','\uEC47\uEC48\uEC49\uEC52','\uEC48\uEC49\uEC4A\uEC52','\uEC46\uEC48\uEC4D\uEC52','\uEC46\uEC4E\uEC4D','\uEC46\uEC47\uEC49\uEC50',</v>
       </c>
     </row>
-    <row r="40" spans="1:26" ht="18" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>29</v>
       </c>
@@ -3293,7 +3272,7 @@
       <c r="X40" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="Y40" s="8" t="str">
+      <c r="Y40" s="3" t="str">
         <f t="shared" si="0"/>
         <v>\uEC47\uEC48\uEC49\uEC4A\uEC4D</v>
       </c>
@@ -3302,7 +3281,7 @@
         <v>'\uEC47\uEC48\uEC49\uEC4A\uEC4D',</v>
       </c>
     </row>
-    <row r="41" spans="1:26" ht="18" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>53</v>
       </c>
@@ -3332,7 +3311,7 @@
       <c r="X41" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="Y41" s="8" t="str">
+      <c r="Y41" s="3" t="str">
         <f t="shared" ref="Y41" si="2">_xlfn.CONCAT(C41:U41)</f>
         <v>\uEC48\uEC4D\uEC51\uEC55\uEC53</v>
       </c>
@@ -3341,7 +3320,7 @@
         <v>'\uEC47\uEC48\uEC49\uEC4A\uEC4D','\uEC48\uEC4D\uEC51\uEC55\uEC53',</v>
       </c>
     </row>
-    <row r="42" spans="1:26" ht="18" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>8</v>
       </c>
@@ -3372,7 +3351,7 @@
       <c r="X42" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="Y42" s="8" t="str">
+      <c r="Y42" s="3" t="str">
         <f t="shared" ref="Y42:Y49" si="3">_xlfn.CONCAT(C42:U42)</f>
         <v>\uEC46\uEC48\uEC49\uEC4D\uEC4F\uEC55</v>
       </c>
@@ -3381,7 +3360,7 @@
         <v>'\uEC47\uEC48\uEC49\uEC4A\uEC4D','\uEC48\uEC4D\uEC51\uEC55\uEC53','\uEC46\uEC48\uEC49\uEC4D\uEC4F\uEC55',</v>
       </c>
     </row>
-    <row r="43" spans="1:26" ht="18" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>54</v>
       </c>
@@ -3412,7 +3391,7 @@
       <c r="X43" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="Y43" s="8" t="str">
+      <c r="Y43" s="3" t="str">
         <f t="shared" si="3"/>
         <v>\uEC46\uEC49\uEC4E\uEC4D\uEC55\uEC53</v>
       </c>
@@ -3421,7 +3400,7 @@
         <v>'\uEC47\uEC48\uEC49\uEC4A\uEC4D','\uEC48\uEC4D\uEC51\uEC55\uEC53','\uEC46\uEC48\uEC49\uEC4D\uEC4F\uEC55','\uEC46\uEC49\uEC4E\uEC4D\uEC55\uEC53',</v>
       </c>
     </row>
-    <row r="44" spans="1:26" ht="18" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>7</v>
       </c>
@@ -3461,7 +3440,7 @@
       <c r="X44" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="Y44" s="8" t="str">
+      <c r="Y44" s="3" t="str">
         <f t="shared" si="3"/>
         <v>\uEC46\uEC48\uEC49\uEC4A\uEC4E\uEC50\uEC51\uEC54\uEC55</v>
       </c>
@@ -3470,7 +3449,7 @@
         <v>'\uEC47\uEC48\uEC49\uEC4A\uEC4D','\uEC48\uEC4D\uEC51\uEC55\uEC53','\uEC46\uEC48\uEC49\uEC4D\uEC4F\uEC55','\uEC46\uEC49\uEC4E\uEC4D\uEC55\uEC53','\uEC46\uEC48\uEC49\uEC4A\uEC4E\uEC50\uEC51\uEC54\uEC55',</v>
       </c>
     </row>
-    <row r="45" spans="1:26" ht="18" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>6</v>
       </c>
@@ -3498,7 +3477,7 @@
       <c r="X45" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="Y45" s="8" t="str">
+      <c r="Y45" s="3" t="str">
         <f t="shared" si="3"/>
         <v>\uEC48\uEC50\uEC51\uEC52\uEC53</v>
       </c>
@@ -3507,7 +3486,7 @@
         <v>'\uEC47\uEC48\uEC49\uEC4A\uEC4D','\uEC48\uEC4D\uEC51\uEC55\uEC53','\uEC46\uEC48\uEC49\uEC4D\uEC4F\uEC55','\uEC46\uEC49\uEC4E\uEC4D\uEC55\uEC53','\uEC46\uEC48\uEC49\uEC4A\uEC4E\uEC50\uEC51\uEC54\uEC55','\uEC48\uEC50\uEC51\uEC52\uEC53',</v>
       </c>
     </row>
-    <row r="46" spans="1:26" ht="18" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>55</v>
       </c>
@@ -3538,7 +3517,7 @@
       <c r="X46" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="Y46" s="8" t="str">
+      <c r="Y46" s="3" t="str">
         <f t="shared" si="3"/>
         <v>\uEC46\uEC4A\uEC4D\uEC51\uEC52\uEC53</v>
       </c>
@@ -3547,7 +3526,7 @@
         <v>'\uEC47\uEC48\uEC49\uEC4A\uEC4D','\uEC48\uEC4D\uEC51\uEC55\uEC53','\uEC46\uEC48\uEC49\uEC4D\uEC4F\uEC55','\uEC46\uEC49\uEC4E\uEC4D\uEC55\uEC53','\uEC46\uEC48\uEC49\uEC4A\uEC4E\uEC50\uEC51\uEC54\uEC55','\uEC48\uEC50\uEC51\uEC52\uEC53','\uEC46\uEC4A\uEC4D\uEC51\uEC52\uEC53',</v>
       </c>
     </row>
-    <row r="47" spans="1:26" ht="18" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>5</v>
       </c>
@@ -3578,7 +3557,7 @@
       <c r="X47" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="Y47" s="8" t="str">
+      <c r="Y47" s="3" t="str">
         <f t="shared" si="3"/>
         <v>\uEC46\uEC48\uEC49\uEC4A\uEC4E\uEC4F</v>
       </c>
@@ -3587,7 +3566,7 @@
         <v>'\uEC47\uEC48\uEC49\uEC4A\uEC4D','\uEC48\uEC4D\uEC51\uEC55\uEC53','\uEC46\uEC48\uEC49\uEC4D\uEC4F\uEC55','\uEC46\uEC49\uEC4E\uEC4D\uEC55\uEC53','\uEC46\uEC48\uEC49\uEC4A\uEC4E\uEC50\uEC51\uEC54\uEC55','\uEC48\uEC50\uEC51\uEC52\uEC53','\uEC46\uEC4A\uEC4D\uEC51\uEC52\uEC53','\uEC46\uEC48\uEC49\uEC4A\uEC4E\uEC4F',</v>
       </c>
     </row>
-    <row r="48" spans="1:26" ht="18" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>56</v>
       </c>
@@ -3630,7 +3609,7 @@
       <c r="X48" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="Y48" s="8" t="str">
+      <c r="Y48" s="3" t="str">
         <f t="shared" si="3"/>
         <v>\uEC46\uEC48\uEC49\uEC4A\uEC4E\uEC4F\uEC51\uEC54\uEC55\uEC53</v>
       </c>
@@ -3639,7 +3618,7 @@
         <v>'\uEC47\uEC48\uEC49\uEC4A\uEC4D','\uEC48\uEC4D\uEC51\uEC55\uEC53','\uEC46\uEC48\uEC49\uEC4D\uEC4F\uEC55','\uEC46\uEC49\uEC4E\uEC4D\uEC55\uEC53','\uEC46\uEC48\uEC49\uEC4A\uEC4E\uEC50\uEC51\uEC54\uEC55','\uEC48\uEC50\uEC51\uEC52\uEC53','\uEC46\uEC4A\uEC4D\uEC51\uEC52\uEC53','\uEC46\uEC48\uEC49\uEC4A\uEC4E\uEC4F','\uEC46\uEC48\uEC49\uEC4A\uEC4E\uEC4F\uEC51\uEC54\uEC55\uEC53',</v>
       </c>
     </row>
-    <row r="49" spans="1:26" ht="18" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>4</v>
       </c>
@@ -3685,7 +3664,7 @@
       <c r="X49" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="Y49" s="8" t="str">
+      <c r="Y49" s="3" t="str">
         <f t="shared" si="3"/>
         <v>\uEC46\uEC48\uEC49\uEC4A\uEC4E\uEC59\uEC4F\uEC51\uEC54\uEC55\uEC53</v>
       </c>
@@ -3694,7 +3673,7 @@
         <v>'\uEC47\uEC48\uEC49\uEC4A\uEC4D','\uEC48\uEC4D\uEC51\uEC55\uEC53','\uEC46\uEC48\uEC49\uEC4D\uEC4F\uEC55','\uEC46\uEC49\uEC4E\uEC4D\uEC55\uEC53','\uEC46\uEC48\uEC49\uEC4A\uEC4E\uEC50\uEC51\uEC54\uEC55','\uEC48\uEC50\uEC51\uEC52\uEC53','\uEC46\uEC4A\uEC4D\uEC51\uEC52\uEC53','\uEC46\uEC48\uEC49\uEC4A\uEC4E\uEC4F','\uEC46\uEC48\uEC49\uEC4A\uEC4E\uEC4F\uEC51\uEC54\uEC55\uEC53','\uEC46\uEC48\uEC49\uEC4A\uEC4E\uEC59\uEC4F\uEC51\uEC54\uEC55\uEC53',</v>
       </c>
     </row>
-    <row r="50" spans="1:26" ht="18" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>57</v>
       </c>
@@ -3707,9 +3686,9 @@
       <c r="X50" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="Y50" s="9"/>
-    </row>
-    <row r="51" spans="1:26" ht="18" x14ac:dyDescent="0.25">
+      <c r="Y50" s="3"/>
+    </row>
+    <row r="51" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>3</v>
       </c>
@@ -3722,9 +3701,9 @@
       <c r="X51" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="Y51" s="9"/>
-    </row>
-    <row r="52" spans="1:26" ht="18" x14ac:dyDescent="0.25">
+      <c r="Y51" s="3"/>
+    </row>
+    <row r="52" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>30</v>
       </c>
@@ -3743,9 +3722,9 @@
       <c r="X52" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="Y52" s="9"/>
-    </row>
-    <row r="53" spans="1:26" ht="18" x14ac:dyDescent="0.25">
+      <c r="Y52" s="3"/>
+    </row>
+    <row r="53" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>58</v>
       </c>
@@ -3758,7 +3737,7 @@
       <c r="X53" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="Y53" s="9"/>
+      <c r="Y53" s="3"/>
     </row>
     <row r="54" spans="1:26" ht="18" x14ac:dyDescent="0.25">
       <c r="Y54" s="9"/>
@@ -10785,13 +10764,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C098320-1ECA-4C4B-B8F4-465E7E7241CA}">
-  <dimension ref="A1:T38"/>
+  <dimension ref="A1:S38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="S36" sqref="S36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10804,10 +10783,11 @@
     <col min="8" max="8" width="8.5" customWidth="1"/>
     <col min="9" max="9" width="9.33203125" customWidth="1"/>
     <col min="10" max="17" width="8.5" customWidth="1"/>
-    <col min="18" max="19" width="24.6640625" customWidth="1"/>
+    <col min="18" max="18" width="24.6640625" customWidth="1"/>
+    <col min="19" max="19" width="19.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>31</v>
       </c>
@@ -10861,13 +10841,10 @@
         <v>152</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="T1" s="1" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B2" s="4"/>
       <c r="C2" s="4" t="s">
         <v>183</v>
@@ -10907,15 +10884,11 @@
       <c r="Q2" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="R2" s="8">
-        <v>60480</v>
-      </c>
-      <c r="S2" t="str">
-        <f>_xlfn.UNICHAR(R2)</f>
-        <v></v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+      <c r="R2" s="4" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -10960,19 +10933,16 @@
       <c r="Q3" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="R3" s="8" t="str">
+      <c r="R3" s="4" t="str">
         <f>_xlfn.CONCAT(C3:N3)</f>
         <v>\uEF61\uEF62\uEF63\uEF64\uEF65\uEF66\uEF67\uEF68\uEF69\uEF6A</v>
       </c>
-      <c r="S3" s="8" t="s">
-        <v>201</v>
-      </c>
-      <c r="T3" t="str">
+      <c r="S3" t="str">
         <f>"'"&amp;R3&amp;"',"</f>
         <v>'\uEF61\uEF62\uEF63\uEF64\uEF65\uEF66\uEF67\uEF68\uEF69\uEF6A',</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -11013,17 +10983,16 @@
       <c r="Q4" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="R4" s="8" t="str">
+      <c r="R4" s="4" t="str">
         <f t="shared" ref="R4:R36" si="0">_xlfn.CONCAT(C4:N4)</f>
         <v>\uEF61\uEF62\uEF63\uEF64\uEF65\uEF66\uEF67\uEF68\uEF69</v>
       </c>
-      <c r="S4" s="8"/>
-      <c r="T4" t="str">
-        <f t="shared" ref="T4:T34" si="1">T3&amp;"'"&amp;R4&amp;"',"</f>
+      <c r="S4" t="str">
+        <f>S3&amp;"'"&amp;R4&amp;"',"</f>
         <v>'\uEF61\uEF62\uEF63\uEF64\uEF65\uEF66\uEF67\uEF68\uEF69\uEF6A','\uEF61\uEF62\uEF63\uEF64\uEF65\uEF66\uEF67\uEF68\uEF69',</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -11061,17 +11030,16 @@
       <c r="Q5" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="R5" s="8" t="str">
+      <c r="R5" s="4" t="str">
         <f t="shared" si="0"/>
         <v>\uEF61\uEF62\uEF63\uEF64\uEF65\uEF66\uEF67\uEF68</v>
       </c>
-      <c r="S5" s="8"/>
-      <c r="T5" t="str">
-        <f t="shared" si="1"/>
+      <c r="S5" t="str">
+        <f>S4&amp;"'"&amp;R5&amp;"',"</f>
         <v>'\uEF61\uEF62\uEF63\uEF64\uEF65\uEF66\uEF67\uEF68\uEF69\uEF6A','\uEF61\uEF62\uEF63\uEF64\uEF65\uEF66\uEF67\uEF68\uEF69','\uEF61\uEF62\uEF63\uEF64\uEF65\uEF66\uEF67\uEF68',</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>44</v>
       </c>
@@ -11106,17 +11074,16 @@
       <c r="Q6" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="R6" s="8" t="str">
+      <c r="R6" s="4" t="str">
         <f t="shared" si="0"/>
         <v>\uEF61\uEF62\uEF63\uEF64\uEF65\uEF66\uEF67</v>
       </c>
-      <c r="S6" s="8"/>
-      <c r="T6" t="str">
-        <f t="shared" si="1"/>
+      <c r="S6" t="str">
+        <f>S5&amp;"'"&amp;R6&amp;"',"</f>
         <v>'\uEF61\uEF62\uEF63\uEF64\uEF65\uEF66\uEF67\uEF68\uEF69\uEF6A','\uEF61\uEF62\uEF63\uEF64\uEF65\uEF66\uEF67\uEF68\uEF69','\uEF61\uEF62\uEF63\uEF64\uEF65\uEF66\uEF67\uEF68','\uEF61\uEF62\uEF63\uEF64\uEF65\uEF66\uEF67',</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -11148,17 +11115,16 @@
       <c r="Q7" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="R7" s="8" t="str">
+      <c r="R7" s="4" t="str">
         <f t="shared" si="0"/>
         <v>\uEF61\uEF62\uEF63\uEF64\uEF65\uEF66</v>
       </c>
-      <c r="S7" s="8"/>
-      <c r="T7" t="str">
-        <f t="shared" si="1"/>
+      <c r="S7" t="str">
+        <f>S6&amp;"'"&amp;R7&amp;"',"</f>
         <v>'\uEF61\uEF62\uEF63\uEF64\uEF65\uEF66\uEF67\uEF68\uEF69\uEF6A','\uEF61\uEF62\uEF63\uEF64\uEF65\uEF66\uEF67\uEF68\uEF69','\uEF61\uEF62\uEF63\uEF64\uEF65\uEF66\uEF67\uEF68','\uEF61\uEF62\uEF63\uEF64\uEF65\uEF66\uEF67','\uEF61\uEF62\uEF63\uEF64\uEF65\uEF66',</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -11199,17 +11165,16 @@
       <c r="Q8" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="R8" s="8" t="str">
+      <c r="R8" s="4" t="str">
         <f t="shared" si="0"/>
         <v>\uEF61\uEF62\uEF63\uEF64\uEF65\uEF67\uEF68\uEF69\uEF6A</v>
       </c>
-      <c r="S8" s="8"/>
-      <c r="T8" t="str">
-        <f t="shared" si="1"/>
+      <c r="S8" t="str">
+        <f>S7&amp;"'"&amp;R8&amp;"',"</f>
         <v>'\uEF61\uEF62\uEF63\uEF64\uEF65\uEF66\uEF67\uEF68\uEF69\uEF6A','\uEF61\uEF62\uEF63\uEF64\uEF65\uEF66\uEF67\uEF68\uEF69','\uEF61\uEF62\uEF63\uEF64\uEF65\uEF66\uEF67\uEF68','\uEF61\uEF62\uEF63\uEF64\uEF65\uEF66\uEF67','\uEF61\uEF62\uEF63\uEF64\uEF65\uEF66','\uEF61\uEF62\uEF63\uEF64\uEF65\uEF67\uEF68\uEF69\uEF6A',</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>45</v>
       </c>
@@ -11243,17 +11208,16 @@
       <c r="Q9" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="R9" s="8" t="str">
+      <c r="R9" s="4" t="str">
         <f t="shared" si="0"/>
         <v>\uEF61\uEF62\uEF63\uEF64\uEF66\uEF67\uEF68</v>
       </c>
-      <c r="S9" s="8"/>
-      <c r="T9" t="str">
-        <f t="shared" si="1"/>
+      <c r="S9" t="str">
+        <f>S8&amp;"'"&amp;R9&amp;"',"</f>
         <v>'\uEF61\uEF62\uEF63\uEF64\uEF65\uEF66\uEF67\uEF68\uEF69\uEF6A','\uEF61\uEF62\uEF63\uEF64\uEF65\uEF66\uEF67\uEF68\uEF69','\uEF61\uEF62\uEF63\uEF64\uEF65\uEF66\uEF67\uEF68','\uEF61\uEF62\uEF63\uEF64\uEF65\uEF66\uEF67','\uEF61\uEF62\uEF63\uEF64\uEF65\uEF66','\uEF61\uEF62\uEF63\uEF64\uEF65\uEF67\uEF68\uEF69\uEF6A','\uEF61\uEF62\uEF63\uEF64\uEF66\uEF67\uEF68',</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -11278,17 +11242,16 @@
       <c r="Q10" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="R10" s="8" t="str">
+      <c r="R10" s="4" t="str">
         <f t="shared" si="0"/>
         <v>\uEF61\uEF62\uEF63\uEF64</v>
       </c>
-      <c r="S10" s="8"/>
-      <c r="T10" t="str">
-        <f t="shared" si="1"/>
+      <c r="S10" t="str">
+        <f>S9&amp;"'"&amp;R10&amp;"',"</f>
         <v>'\uEF61\uEF62\uEF63\uEF64\uEF65\uEF66\uEF67\uEF68\uEF69\uEF6A','\uEF61\uEF62\uEF63\uEF64\uEF65\uEF66\uEF67\uEF68\uEF69','\uEF61\uEF62\uEF63\uEF64\uEF65\uEF66\uEF67\uEF68','\uEF61\uEF62\uEF63\uEF64\uEF65\uEF66\uEF67','\uEF61\uEF62\uEF63\uEF64\uEF65\uEF66','\uEF61\uEF62\uEF63\uEF64\uEF65\uEF67\uEF68\uEF69\uEF6A','\uEF61\uEF62\uEF63\uEF64\uEF66\uEF67\uEF68','\uEF61\uEF62\uEF63\uEF64',</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>46</v>
       </c>
@@ -11319,17 +11282,16 @@
       <c r="Q11" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="R11" s="8" t="str">
+      <c r="R11" s="4" t="str">
         <f t="shared" si="0"/>
         <v>\uEF61\uEF62\uEF63\uEF65\uEF66\uEF67</v>
       </c>
-      <c r="S11" s="8"/>
-      <c r="T11" t="str">
-        <f t="shared" si="1"/>
+      <c r="S11" t="str">
+        <f>S10&amp;"'"&amp;R11&amp;"',"</f>
         <v>'\uEF61\uEF62\uEF63\uEF64\uEF65\uEF66\uEF67\uEF68\uEF69\uEF6A','\uEF61\uEF62\uEF63\uEF64\uEF65\uEF66\uEF67\uEF68\uEF69','\uEF61\uEF62\uEF63\uEF64\uEF65\uEF66\uEF67\uEF68','\uEF61\uEF62\uEF63\uEF64\uEF65\uEF66\uEF67','\uEF61\uEF62\uEF63\uEF64\uEF65\uEF66','\uEF61\uEF62\uEF63\uEF64\uEF65\uEF67\uEF68\uEF69\uEF6A','\uEF61\uEF62\uEF63\uEF64\uEF66\uEF67\uEF68','\uEF61\uEF62\uEF63\uEF64','\uEF61\uEF62\uEF63\uEF65\uEF66\uEF67',</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -11351,17 +11313,16 @@
       <c r="Q12" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="R12" s="8" t="str">
+      <c r="R12" s="4" t="str">
         <f t="shared" si="0"/>
         <v>\uEF61\uEF62\uEF63</v>
       </c>
-      <c r="S12" s="8"/>
-      <c r="T12" t="str">
-        <f t="shared" si="1"/>
+      <c r="S12" t="str">
+        <f>S11&amp;"'"&amp;R12&amp;"',"</f>
         <v>'\uEF61\uEF62\uEF63\uEF64\uEF65\uEF66\uEF67\uEF68\uEF69\uEF6A','\uEF61\uEF62\uEF63\uEF64\uEF65\uEF66\uEF67\uEF68\uEF69','\uEF61\uEF62\uEF63\uEF64\uEF65\uEF66\uEF67\uEF68','\uEF61\uEF62\uEF63\uEF64\uEF65\uEF66\uEF67','\uEF61\uEF62\uEF63\uEF64\uEF65\uEF66','\uEF61\uEF62\uEF63\uEF64\uEF65\uEF67\uEF68\uEF69\uEF6A','\uEF61\uEF62\uEF63\uEF64\uEF66\uEF67\uEF68','\uEF61\uEF62\uEF63\uEF64','\uEF61\uEF62\uEF63\uEF65\uEF66\uEF67','\uEF61\uEF62\uEF63',</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>47</v>
       </c>
@@ -11386,17 +11347,16 @@
       <c r="Q13" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="R13" s="8" t="str">
+      <c r="R13" s="4" t="str">
         <f t="shared" si="0"/>
         <v>\uEF61\uEF62\uEF64\uEF65</v>
       </c>
-      <c r="S13" s="8"/>
-      <c r="T13" t="str">
-        <f t="shared" si="1"/>
+      <c r="S13" t="str">
+        <f>S12&amp;"'"&amp;R13&amp;"',"</f>
         <v>'\uEF61\uEF62\uEF63\uEF64\uEF65\uEF66\uEF67\uEF68\uEF69\uEF6A','\uEF61\uEF62\uEF63\uEF64\uEF65\uEF66\uEF67\uEF68\uEF69','\uEF61\uEF62\uEF63\uEF64\uEF65\uEF66\uEF67\uEF68','\uEF61\uEF62\uEF63\uEF64\uEF65\uEF66\uEF67','\uEF61\uEF62\uEF63\uEF64\uEF65\uEF66','\uEF61\uEF62\uEF63\uEF64\uEF65\uEF67\uEF68\uEF69\uEF6A','\uEF61\uEF62\uEF63\uEF64\uEF66\uEF67\uEF68','\uEF61\uEF62\uEF63\uEF64','\uEF61\uEF62\uEF63\uEF65\uEF66\uEF67','\uEF61\uEF62\uEF63','\uEF61\uEF62\uEF64\uEF65',</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -11415,17 +11375,16 @@
       <c r="Q14" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="R14" s="8" t="str">
+      <c r="R14" s="4" t="str">
         <f t="shared" si="0"/>
         <v>\uEF61\uEF62</v>
       </c>
-      <c r="S14" s="8"/>
-      <c r="T14" t="str">
-        <f t="shared" si="1"/>
+      <c r="S14" t="str">
+        <f>S13&amp;"'"&amp;R14&amp;"',"</f>
         <v>'\uEF61\uEF62\uEF63\uEF64\uEF65\uEF66\uEF67\uEF68\uEF69\uEF6A','\uEF61\uEF62\uEF63\uEF64\uEF65\uEF66\uEF67\uEF68\uEF69','\uEF61\uEF62\uEF63\uEF64\uEF65\uEF66\uEF67\uEF68','\uEF61\uEF62\uEF63\uEF64\uEF65\uEF66\uEF67','\uEF61\uEF62\uEF63\uEF64\uEF65\uEF66','\uEF61\uEF62\uEF63\uEF64\uEF65\uEF67\uEF68\uEF69\uEF6A','\uEF61\uEF62\uEF63\uEF64\uEF66\uEF67\uEF68','\uEF61\uEF62\uEF63\uEF64','\uEF61\uEF62\uEF63\uEF65\uEF66\uEF67','\uEF61\uEF62\uEF63','\uEF61\uEF62\uEF64\uEF65','\uEF61\uEF62',</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -11455,17 +11414,16 @@
       <c r="Q15" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="R15" s="8" t="str">
+      <c r="R15" s="4" t="str">
         <f t="shared" si="0"/>
         <v>\uEF61\uEF63</v>
       </c>
-      <c r="S15" s="8"/>
-      <c r="T15" t="str">
+      <c r="S15" t="str">
         <f>"'"&amp;R15&amp;"',"</f>
         <v>'\uEF61\uEF63',</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>48</v>
       </c>
@@ -11495,17 +11453,16 @@
       <c r="Q16" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="R16" s="8" t="str">
+      <c r="R16" s="4" t="str">
         <f t="shared" si="0"/>
         <v>\uEF62\uEF63</v>
       </c>
-      <c r="S16" s="8"/>
-      <c r="T16" t="str">
-        <f t="shared" si="1"/>
+      <c r="S16" t="str">
+        <f>S15&amp;"'"&amp;R16&amp;"',"</f>
         <v>'\uEF61\uEF63','\uEF62\uEF63',</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -11533,17 +11490,16 @@
       <c r="Q17" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="R17" s="8" t="str">
+      <c r="R17" s="4" t="str">
         <f t="shared" si="0"/>
         <v>\uEF63</v>
       </c>
-      <c r="S17" s="8"/>
-      <c r="T17" t="str">
-        <f t="shared" si="1"/>
+      <c r="S17" t="str">
+        <f>S16&amp;"'"&amp;R17&amp;"',"</f>
         <v>'\uEF61\uEF63','\uEF62\uEF63','\uEF63',</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>49</v>
       </c>
@@ -11581,17 +11537,16 @@
       <c r="Q18" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="R18" s="8" t="str">
+      <c r="R18" s="4" t="str">
         <f t="shared" si="0"/>
         <v>\uEF63\uEF64\uEF65\uEF66\uEF67\uEF68</v>
       </c>
-      <c r="S18" s="8"/>
-      <c r="T18" t="str">
-        <f t="shared" si="1"/>
+      <c r="S18" t="str">
+        <f>S17&amp;"'"&amp;R18&amp;"',"</f>
         <v>'\uEF61\uEF63','\uEF62\uEF63','\uEF63','\uEF63\uEF64\uEF65\uEF66\uEF67\uEF68',</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -11629,17 +11584,16 @@
       <c r="Q19" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="R19" s="8" t="str">
+      <c r="R19" s="4" t="str">
         <f t="shared" si="0"/>
         <v>\uEF6B\uEF62\uEF63\uEF64\uEF65\uEF66</v>
       </c>
-      <c r="S19" s="8"/>
-      <c r="T19" t="str">
-        <f t="shared" si="1"/>
+      <c r="S19" t="str">
+        <f>S18&amp;"'"&amp;R19&amp;"',"</f>
         <v>'\uEF61\uEF63','\uEF62\uEF63','\uEF63','\uEF63\uEF64\uEF65\uEF66\uEF67\uEF68','\uEF6B\uEF62\uEF63\uEF64\uEF65\uEF66',</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -11679,17 +11633,16 @@
       <c r="Q20" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="R20" s="8" t="str">
+      <c r="R20" s="4" t="str">
         <f t="shared" si="0"/>
         <v>\uEF6B\uEF62\uEF63\uEF64\uEF65\uEF67\uEF68</v>
       </c>
-      <c r="S20" s="8"/>
-      <c r="T20" t="str">
-        <f t="shared" si="1"/>
+      <c r="S20" t="str">
+        <f>S19&amp;"'"&amp;R20&amp;"',"</f>
         <v>'\uEF61\uEF63','\uEF62\uEF63','\uEF63','\uEF63\uEF64\uEF65\uEF66\uEF67\uEF68','\uEF6B\uEF62\uEF63\uEF64\uEF65\uEF66','\uEF6B\uEF62\uEF63\uEF64\uEF65\uEF67\uEF68',</v>
       </c>
     </row>
-    <row r="21" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>50</v>
       </c>
@@ -11725,17 +11678,16 @@
       <c r="Q21" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="R21" s="8" t="str">
+      <c r="R21" s="4" t="str">
         <f t="shared" si="0"/>
         <v>\uEF6B\uEF62\uEF63\uEF64\uEF66</v>
       </c>
-      <c r="S21" s="8"/>
-      <c r="T21" t="str">
-        <f t="shared" si="1"/>
+      <c r="S21" t="str">
+        <f>S20&amp;"'"&amp;R21&amp;"',"</f>
         <v>'\uEF61\uEF63','\uEF62\uEF63','\uEF63','\uEF63\uEF64\uEF65\uEF66\uEF67\uEF68','\uEF6B\uEF62\uEF63\uEF64\uEF65\uEF66','\uEF6B\uEF62\uEF63\uEF64\uEF65\uEF67\uEF68','\uEF6B\uEF62\uEF63\uEF64\uEF66',</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>11</v>
       </c>
@@ -11769,17 +11721,16 @@
       <c r="Q22" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="R22" s="8" t="str">
+      <c r="R22" s="4" t="str">
         <f t="shared" si="0"/>
         <v>\uEF6B\uEF62\uEF63\uEF64</v>
       </c>
-      <c r="S22" s="8"/>
-      <c r="T22" t="str">
-        <f t="shared" si="1"/>
+      <c r="S22" t="str">
+        <f>S21&amp;"'"&amp;R22&amp;"',"</f>
         <v>'\uEF61\uEF63','\uEF62\uEF63','\uEF63','\uEF63\uEF64\uEF65\uEF66\uEF67\uEF68','\uEF6B\uEF62\uEF63\uEF64\uEF65\uEF66','\uEF6B\uEF62\uEF63\uEF64\uEF65\uEF67\uEF68','\uEF6B\uEF62\uEF63\uEF64\uEF66','\uEF6B\uEF62\uEF63\uEF64',</v>
       </c>
     </row>
-    <row r="23" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>51</v>
       </c>
@@ -11813,17 +11764,16 @@
       <c r="Q23" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="R23" s="8" t="str">
+      <c r="R23" s="4" t="str">
         <f t="shared" si="0"/>
         <v>\uEF6B\uEF62\uEF63\uEF65</v>
       </c>
-      <c r="S23" s="8"/>
-      <c r="T23" t="str">
-        <f t="shared" si="1"/>
+      <c r="S23" t="str">
+        <f>S22&amp;"'"&amp;R23&amp;"',"</f>
         <v>'\uEF61\uEF63','\uEF62\uEF63','\uEF63','\uEF63\uEF64\uEF65\uEF66\uEF67\uEF68','\uEF6B\uEF62\uEF63\uEF64\uEF65\uEF66','\uEF6B\uEF62\uEF63\uEF64\uEF65\uEF67\uEF68','\uEF6B\uEF62\uEF63\uEF64\uEF66','\uEF6B\uEF62\uEF63\uEF64','\uEF6B\uEF62\uEF63\uEF65',</v>
       </c>
     </row>
-    <row r="24" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>10</v>
       </c>
@@ -11855,17 +11805,16 @@
       <c r="Q24" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="R24" s="8" t="str">
+      <c r="R24" s="4" t="str">
         <f t="shared" si="0"/>
         <v>\uEF6B\uEF62\uEF63</v>
       </c>
-      <c r="S24" s="8"/>
-      <c r="T24" t="str">
-        <f t="shared" si="1"/>
+      <c r="S24" t="str">
+        <f>S23&amp;"'"&amp;R24&amp;"',"</f>
         <v>'\uEF61\uEF63','\uEF62\uEF63','\uEF63','\uEF63\uEF64\uEF65\uEF66\uEF67\uEF68','\uEF6B\uEF62\uEF63\uEF64\uEF65\uEF66','\uEF6B\uEF62\uEF63\uEF64\uEF65\uEF67\uEF68','\uEF6B\uEF62\uEF63\uEF64\uEF66','\uEF6B\uEF62\uEF63\uEF64','\uEF6B\uEF62\uEF63\uEF65','\uEF6B\uEF62\uEF63',</v>
       </c>
     </row>
-    <row r="25" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>52</v>
       </c>
@@ -11903,17 +11852,16 @@
       <c r="Q25" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="R25" s="8" t="str">
+      <c r="R25" s="4" t="str">
         <f t="shared" si="0"/>
         <v>\uEF6B\uEF62\uEF63\uEF66\uEF67\uEF68</v>
       </c>
-      <c r="S25" s="8"/>
-      <c r="T25" t="str">
-        <f t="shared" si="1"/>
+      <c r="S25" t="str">
+        <f>S24&amp;"'"&amp;R25&amp;"',"</f>
         <v>'\uEF61\uEF63','\uEF62\uEF63','\uEF63','\uEF63\uEF64\uEF65\uEF66\uEF67\uEF68','\uEF6B\uEF62\uEF63\uEF64\uEF65\uEF66','\uEF6B\uEF62\uEF63\uEF64\uEF65\uEF67\uEF68','\uEF6B\uEF62\uEF63\uEF64\uEF66','\uEF6B\uEF62\uEF63\uEF64','\uEF6B\uEF62\uEF63\uEF65','\uEF6B\uEF62\uEF63','\uEF6B\uEF62\uEF63\uEF66\uEF67\uEF68',</v>
       </c>
     </row>
-    <row r="26" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>9</v>
       </c>
@@ -11949,17 +11897,16 @@
       <c r="Q26" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="R26" s="8" t="str">
+      <c r="R26" s="4" t="str">
         <f t="shared" si="0"/>
         <v>\uEF6B\uEF62\uEF63\uEF65\uEF66</v>
       </c>
-      <c r="S26" s="8"/>
-      <c r="T26" t="str">
-        <f t="shared" si="1"/>
+      <c r="S26" t="str">
+        <f>S25&amp;"'"&amp;R26&amp;"',"</f>
         <v>'\uEF61\uEF63','\uEF62\uEF63','\uEF63','\uEF63\uEF64\uEF65\uEF66\uEF67\uEF68','\uEF6B\uEF62\uEF63\uEF64\uEF65\uEF66','\uEF6B\uEF62\uEF63\uEF64\uEF65\uEF67\uEF68','\uEF6B\uEF62\uEF63\uEF64\uEF66','\uEF6B\uEF62\uEF63\uEF64','\uEF6B\uEF62\uEF63\uEF65','\uEF6B\uEF62\uEF63','\uEF6B\uEF62\uEF63\uEF66\uEF67\uEF68','\uEF6B\uEF62\uEF63\uEF65\uEF66',</v>
       </c>
     </row>
-    <row r="27" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>29</v>
       </c>
@@ -11993,17 +11940,16 @@
       <c r="Q27" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="R27" s="8" t="str">
+      <c r="R27" s="4" t="str">
         <f t="shared" si="0"/>
         <v>\uEF6B\uEF62\uEF65\uEF66</v>
       </c>
-      <c r="S27" s="8"/>
-      <c r="T27" t="str">
+      <c r="S27" t="str">
         <f>"'"&amp;R27&amp;"',"</f>
         <v>'\uEF6B\uEF62\uEF65\uEF66',</v>
       </c>
     </row>
-    <row r="28" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>53</v>
       </c>
@@ -12043,17 +11989,16 @@
       <c r="Q28" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="R28" s="8" t="str">
+      <c r="R28" s="4" t="str">
         <f t="shared" si="0"/>
         <v>\uEF6B\uEF62\uEF64\uEF65\uEF67\uEF68\uEF9D</v>
       </c>
-      <c r="S28" s="8"/>
-      <c r="T28" t="str">
-        <f t="shared" si="1"/>
+      <c r="S28" t="str">
+        <f>S27&amp;"'"&amp;R28&amp;"',"</f>
         <v>'\uEF6B\uEF62\uEF65\uEF66','\uEF6B\uEF62\uEF64\uEF65\uEF67\uEF68\uEF9D',</v>
       </c>
     </row>
-    <row r="29" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>8</v>
       </c>
@@ -12091,17 +12036,16 @@
       <c r="Q29" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="R29" s="8" t="str">
+      <c r="R29" s="4" t="str">
         <f t="shared" si="0"/>
         <v>\uEF6B\uEF62\uEF64\uEF65\uEF67\uEF68</v>
       </c>
-      <c r="S29" s="8"/>
-      <c r="T29" t="str">
-        <f t="shared" si="1"/>
+      <c r="S29" t="str">
+        <f>S28&amp;"'"&amp;R29&amp;"',"</f>
         <v>'\uEF6B\uEF62\uEF65\uEF66','\uEF6B\uEF62\uEF64\uEF65\uEF67\uEF68\uEF9D','\uEF6B\uEF62\uEF64\uEF65\uEF67\uEF68',</v>
       </c>
     </row>
-    <row r="30" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>54</v>
       </c>
@@ -12139,17 +12083,16 @@
       <c r="Q30" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="R30" s="8" t="str">
+      <c r="R30" s="4" t="str">
         <f t="shared" si="0"/>
         <v>\uEF6B\uEF63\uEF64\uEF66\uEF67\uEF68</v>
       </c>
-      <c r="S30" s="8"/>
-      <c r="T30" t="str">
-        <f t="shared" si="1"/>
+      <c r="S30" t="str">
+        <f>S29&amp;"'"&amp;R30&amp;"',"</f>
         <v>'\uEF6B\uEF62\uEF65\uEF66','\uEF6B\uEF62\uEF64\uEF65\uEF67\uEF68\uEF9D','\uEF6B\uEF62\uEF64\uEF65\uEF67\uEF68','\uEF6B\uEF63\uEF64\uEF66\uEF67\uEF68',</v>
       </c>
     </row>
-    <row r="31" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>7</v>
       </c>
@@ -12189,17 +12132,16 @@
       <c r="Q31" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="R31" s="8" t="str">
+      <c r="R31" s="4" t="str">
         <f t="shared" si="0"/>
         <v>\uEF6B\uEF63\uEF64\uEF66\uEF67\uEF68\uEF9D</v>
       </c>
-      <c r="S31" s="8"/>
-      <c r="T31" t="str">
-        <f t="shared" si="1"/>
+      <c r="S31" t="str">
+        <f>S30&amp;"'"&amp;R31&amp;"',"</f>
         <v>'\uEF6B\uEF62\uEF65\uEF66','\uEF6B\uEF62\uEF64\uEF65\uEF67\uEF68\uEF9D','\uEF6B\uEF62\uEF64\uEF65\uEF67\uEF68','\uEF6B\uEF63\uEF64\uEF66\uEF67\uEF68','\uEF6B\uEF63\uEF64\uEF66\uEF67\uEF68\uEF9D',</v>
       </c>
     </row>
-    <row r="32" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>6</v>
       </c>
@@ -12237,17 +12179,16 @@
       <c r="Q32" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="R32" s="8" t="str">
+      <c r="R32" s="4" t="str">
         <f t="shared" si="0"/>
         <v>\uEF6B\uEF62\uEF63\uEF65\uEF66\uEF9D</v>
       </c>
-      <c r="S32" s="8"/>
-      <c r="T32" t="str">
-        <f t="shared" si="1"/>
+      <c r="S32" t="str">
+        <f>S31&amp;"'"&amp;R32&amp;"',"</f>
         <v>'\uEF6B\uEF62\uEF65\uEF66','\uEF6B\uEF62\uEF64\uEF65\uEF67\uEF68\uEF9D','\uEF6B\uEF62\uEF64\uEF65\uEF67\uEF68','\uEF6B\uEF63\uEF64\uEF66\uEF67\uEF68','\uEF6B\uEF63\uEF64\uEF66\uEF67\uEF68\uEF9D','\uEF6B\uEF62\uEF63\uEF65\uEF66\uEF9D',</v>
       </c>
     </row>
-    <row r="33" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>55</v>
       </c>
@@ -12283,17 +12224,16 @@
       <c r="Q33" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="R33" s="8" t="str">
+      <c r="R33" s="4" t="str">
         <f t="shared" si="0"/>
         <v>\uEF6B\uEF62\uEF63\uEF65\uEF66</v>
       </c>
-      <c r="S33" s="8"/>
-      <c r="T33" t="str">
-        <f t="shared" si="1"/>
+      <c r="S33" t="str">
+        <f>S32&amp;"'"&amp;R33&amp;"',"</f>
         <v>'\uEF6B\uEF62\uEF65\uEF66','\uEF6B\uEF62\uEF64\uEF65\uEF67\uEF68\uEF9D','\uEF6B\uEF62\uEF64\uEF65\uEF67\uEF68','\uEF6B\uEF63\uEF64\uEF66\uEF67\uEF68','\uEF6B\uEF63\uEF64\uEF66\uEF67\uEF68\uEF9D','\uEF6B\uEF62\uEF63\uEF65\uEF66\uEF9D','\uEF6B\uEF62\uEF63\uEF65\uEF66',</v>
       </c>
     </row>
-    <row r="34" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>5</v>
       </c>
@@ -12325,17 +12265,16 @@
       <c r="Q34" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="R34" s="8" t="str">
+      <c r="R34" s="4" t="str">
         <f t="shared" si="0"/>
         <v>\uEF6B\uEF62\uEF65</v>
       </c>
-      <c r="S34" s="8"/>
-      <c r="T34" t="str">
-        <f t="shared" si="1"/>
+      <c r="S34" t="str">
+        <f>S33&amp;"'"&amp;R34&amp;"',"</f>
         <v>'\uEF6B\uEF62\uEF65\uEF66','\uEF6B\uEF62\uEF64\uEF65\uEF67\uEF68\uEF9D','\uEF6B\uEF62\uEF64\uEF65\uEF67\uEF68','\uEF6B\uEF63\uEF64\uEF66\uEF67\uEF68','\uEF6B\uEF63\uEF64\uEF66\uEF67\uEF68\uEF9D','\uEF6B\uEF62\uEF63\uEF65\uEF66\uEF9D','\uEF6B\uEF62\uEF63\uEF65\uEF66','\uEF6B\uEF62\uEF65',</v>
       </c>
     </row>
-    <row r="35" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>56</v>
       </c>
@@ -12377,17 +12316,16 @@
       <c r="Q35" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="R35" s="8" t="str">
+      <c r="R35" s="4" t="str">
         <f>_xlfn.CONCAT(C35:N35)</f>
         <v>\uEF6B\uEF62\uEF64\uEF67\uEF68\uEF69\uEF6A\uEF9D</v>
       </c>
-      <c r="S35" s="8"/>
-      <c r="T35" t="str">
-        <f t="shared" ref="T35:T36" si="2">T34&amp;"'"&amp;R35&amp;"',"</f>
+      <c r="S35" t="str">
+        <f>S34&amp;"'"&amp;R35&amp;"',"</f>
         <v>'\uEF6B\uEF62\uEF65\uEF66','\uEF6B\uEF62\uEF64\uEF65\uEF67\uEF68\uEF9D','\uEF6B\uEF62\uEF64\uEF65\uEF67\uEF68','\uEF6B\uEF63\uEF64\uEF66\uEF67\uEF68','\uEF6B\uEF63\uEF64\uEF66\uEF67\uEF68\uEF9D','\uEF6B\uEF62\uEF63\uEF65\uEF66\uEF9D','\uEF6B\uEF62\uEF63\uEF65\uEF66','\uEF6B\uEF62\uEF65','\uEF6B\uEF62\uEF64\uEF67\uEF68\uEF69\uEF6A\uEF9D',</v>
       </c>
     </row>
-    <row r="36" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>4</v>
       </c>
@@ -12409,8 +12347,12 @@
       <c r="I36" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="J36" s="11"/>
-      <c r="K36" s="11"/>
+      <c r="J36" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="K36" s="11" t="s">
+        <v>190</v>
+      </c>
       <c r="L36" s="11"/>
       <c r="M36" s="11"/>
       <c r="N36" s="11"/>
@@ -12421,17 +12363,16 @@
       <c r="Q36" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="R36" s="8" t="str">
+      <c r="R36" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>\uEF6B\uEF62\uEF64\uEF66</v>
-      </c>
-      <c r="S36" s="8"/>
-      <c r="T36" t="str">
-        <f t="shared" si="2"/>
-        <v>'\uEF6B\uEF62\uEF65\uEF66','\uEF6B\uEF62\uEF64\uEF65\uEF67\uEF68\uEF9D','\uEF6B\uEF62\uEF64\uEF65\uEF67\uEF68','\uEF6B\uEF63\uEF64\uEF66\uEF67\uEF68','\uEF6B\uEF63\uEF64\uEF66\uEF67\uEF68\uEF9D','\uEF6B\uEF62\uEF63\uEF65\uEF66\uEF9D','\uEF6B\uEF62\uEF63\uEF65\uEF66','\uEF6B\uEF62\uEF65','\uEF6B\uEF62\uEF64\uEF67\uEF68\uEF69\uEF6A\uEF9D','\uEF6B\uEF62\uEF64\uEF66',</v>
-      </c>
-    </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
+        <v>\uEF6B\uEF62\uEF64\uEF66\uEF67\uEF68</v>
+      </c>
+      <c r="S36" t="str">
+        <f>S35&amp;"'"&amp;R36&amp;"',"</f>
+        <v>'\uEF6B\uEF62\uEF65\uEF66','\uEF6B\uEF62\uEF64\uEF65\uEF67\uEF68\uEF9D','\uEF6B\uEF62\uEF64\uEF65\uEF67\uEF68','\uEF6B\uEF63\uEF64\uEF66\uEF67\uEF68','\uEF6B\uEF63\uEF64\uEF66\uEF67\uEF68\uEF9D','\uEF6B\uEF62\uEF63\uEF65\uEF66\uEF9D','\uEF6B\uEF62\uEF63\uEF65\uEF66','\uEF6B\uEF62\uEF65','\uEF6B\uEF62\uEF64\uEF67\uEF68\uEF69\uEF6A\uEF9D','\uEF6B\uEF62\uEF64\uEF66\uEF67\uEF68',</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.2">
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
@@ -12446,7 +12387,7 @@
       <c r="N37" s="6"/>
       <c r="O37" s="6"/>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.2">
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>

</xml_diff>